<commit_message>
Feat: update docs (#2029)
* update in docs, update resources for data model 3.x
</commit_message>
<xml_diff>
--- a/docs/resources/TargetDictionary.xlsx
+++ b/docs/resources/TargetDictionary.xlsx
@@ -1,32 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD39DAFC-CCE4-4264-8640-D8570C040901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBB2195-0298-4393-B45B-7765C0B7D642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TargetDataDictionaries" sheetId="6" r:id="rId1"/>
-    <sheet name="TargetTables" sheetId="7" r:id="rId2"/>
-    <sheet name="TargetVariables" sheetId="9" r:id="rId3"/>
-    <sheet name="RepeatedTargetVariables" sheetId="10" r:id="rId4"/>
-    <sheet name="TargetVariableValues" sheetId="11" r:id="rId5"/>
-    <sheet name="CollectionEvents" sheetId="5" r:id="rId6"/>
-    <sheet name="Subcohorts" sheetId="4" r:id="rId7"/>
+    <sheet name="Datasets" sheetId="7" r:id="rId1"/>
+    <sheet name="Variables" sheetId="9" r:id="rId2"/>
+    <sheet name="Repeated variables" sheetId="10" r:id="rId3"/>
+    <sheet name="Variable values" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -37,98 +34,108 @@
     <t>description</t>
   </si>
   <si>
-    <t>ageGroups</t>
-  </si>
-  <si>
-    <t>disease</t>
-  </si>
-  <si>
-    <t>inclusionCriteria</t>
-  </si>
-  <si>
-    <t>countries</t>
-  </si>
-  <si>
-    <t>regions</t>
-  </si>
-  <si>
-    <t>supplementaryInformation</t>
-  </si>
-  <si>
-    <t>subcohorts</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
     <t>keywords</t>
   </si>
   <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>collectionEvent.resource</t>
-  </si>
-  <si>
-    <t>collectionEvent.name</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
     <t>unit</t>
   </si>
   <si>
-    <t>mandatory</t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
-    <t>exampleValues</t>
-  </si>
-  <si>
     <t>vocabularies</t>
   </si>
   <si>
-    <t>isRepeatOf.table</t>
-  </si>
-  <si>
-    <t>isRepeatOf.name</t>
-  </si>
-  <si>
-    <t>variable.table</t>
-  </si>
-  <si>
     <t>variable.name</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
-    <t>isMissing</t>
-  </si>
-  <si>
-    <t>ontologyTermIRI</t>
-  </si>
-  <si>
-    <t>dataDictionary.resource</t>
-  </si>
-  <si>
-    <t>dataDictionary.version</t>
+    <t>unit of observation</t>
+  </si>
+  <si>
+    <t>number of rows</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>example values</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>collection event.resource</t>
+  </si>
+  <si>
+    <t>collection event.name</t>
+  </si>
+  <si>
+    <t>permitted values</t>
+  </si>
+  <si>
+    <t>repeats</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>since version</t>
+  </si>
+  <si>
+    <t>until version</t>
+  </si>
+  <si>
+    <t>is repeat of.dataset</t>
+  </si>
+  <si>
+    <t>is repeat of.name</t>
+  </si>
+  <si>
+    <t>variable.dataset</t>
+  </si>
+  <si>
+    <t>is missing</t>
+  </si>
+  <si>
+    <t>ontology term URI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,8 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,60 +478,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.31640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.76953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="230.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -531,275 +619,113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.58984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.2265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.58984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.76953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
+    <col min="3" max="3" width="10.06640625" customWidth="1"/>
+    <col min="4" max="4" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="20.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.2265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.04296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.58984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.2265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" t="s">
         <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>